<commit_message>
Mostrar los recursos y los tutores, comparar el puntaje
Se implementaron los métodos que permiten mostrar los recursos, los tutores y comparar el puntaje con el de otros usuarios
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedropablo/Downloads/Proyecto-Final-POO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F1DB37-7A4D-5C4B-BF37-1089D4029FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88E9432-63D0-054F-A9BF-DF03B0266620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{97532FB7-5E9C-4D46-B6D0-317D2D2D62BA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Resource</t>
   </si>
@@ -45,6 +45,27 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Matematica</t>
+  </si>
+  <si>
+    <t>Precalculo 1</t>
+  </si>
+  <si>
+    <t>Calculo 1</t>
+  </si>
+  <si>
+    <t>Ciencias de la vida</t>
+  </si>
+  <si>
+    <t>Ciencias</t>
+  </si>
+  <si>
+    <t>Lenguaje 1</t>
+  </si>
+  <si>
+    <t>Lenguaje</t>
   </si>
 </sst>
 </file>
@@ -80,8 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC4A98C-1D9E-A249-9401-4777125FE048}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,6 +439,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>